<commit_message>
edit list del try catch
</commit_message>
<xml_diff>
--- a/documentlists.xlsx
+++ b/documentlists.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,139 +453,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>128aWGdIIIbDJuMrJM4r8xnYqS5_Ml-wd</t>
+          <t>1GfNKZ05YpkiAeWRb2OS9o_wR3lkRoeER</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>space rent</t>
+          <t>การเลือกซื้อและการเปลี่ยนยางรถยนต์.pdf</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1KRkAFjVeAqy-GSQ3iuXEbw3CdWOPfQUV</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Project Wireframes</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1yKGrWYEgVKiQ1FaYgmZBRZDO4tuLXV4dAc5MAs6J4P0</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ข้อกำหนดความต้องการระบบ</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>10o8Dythbi6_jdvQB4fZqWr0NVRQ-w1NuWxYz5ssGeeI</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>BP payment</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>19oek9KqMVIbWT1VQBt2l5d1sInMkqokT</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BP Register </t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1GpHqxD3Nz4Nou3TLg4BACidn0-bcEnb6</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Untitled Diagram.drawio</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1VxgF2YFF9UJt88u2LLJAvHUkMS4G2OLt</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>software requirement specification</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>1da3Ut5J4nD3dV-__tKvYn4EDFLEjBSWhp3fjsTX0fIk</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Slide-for-training-Govt_12-27-Mar-2018_final-2.pdf</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>1NwcIc5oyD9f1HPHCO1E6bb5jq4idprgw</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>software requirement specification.pdf</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>1FSok90Zy7XWcZGFuK09JX_eLFwVJR5oF</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>4a46371925dd3da5279a773dfb01d33b.pdf</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>1l9FtdJCwM8muQoPsgAJvdtR4x3zrxXFF</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>table of rent system</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>19pl-gUAbT2pcdVZOK7t-skEXclNb4qyLMAO2hs3MfJY</t>
+          <t>1lcVcRis5-qZayIRFJsadxno6jWq9YVir</t>
         </is>
       </c>
     </row>

</xml_diff>